<commit_message>
Updated E2E and Validation Test Case
</commit_message>
<xml_diff>
--- a/testdata/OculusTestData.xlsx
+++ b/testdata/OculusTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Name of Field</t>
   </si>
@@ -130,6 +130,24 @@
   </si>
   <si>
     <t>Your appointment request has been received. Someone from our team at SOUTHWEST CARDIAC ASSOCIATES will be in contact with you shortly to confirm the appointment.</t>
+  </si>
+  <si>
+    <t>Invalid Date Error</t>
+  </si>
+  <si>
+    <t>date must be a `date` type, but the final value was: `Invalid Date`.</t>
+  </si>
+  <si>
+    <t>Invalid Visit Reason</t>
+  </si>
+  <si>
+    <t>Field is required</t>
+  </si>
+  <si>
+    <t>Invalid Birthdate</t>
+  </si>
+  <si>
+    <t>birthdate must be a `date` type, but the final value was: `Invalid Date`.</t>
   </si>
 </sst>
 </file>
@@ -467,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +659,30 @@
         <v>36</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1"/>

</xml_diff>